<commit_message>
added list of abbreviation to roman pages
</commit_message>
<xml_diff>
--- a/data/timestamps.xlsx
+++ b/data/timestamps.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cosmo/Documents/thesis/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFFA83CC-3EE8-BC46-A9F7-3EDAB74E27DE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5F71C8F-E95E-4D41-8B70-DF204F7A501A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{BF4672B2-F65A-AF46-9E75-DFF07DADA656}"/>
   </bookViews>
@@ -383,6 +383,55 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>749300</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>215900</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>355600</xdr:colOff>
+      <xdr:row>78</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{64DF3BAA-FA95-5B48-A98A-2803FB683FA9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10248900" y="3314700"/>
+          <a:ext cx="5384800" cy="16078200"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -685,7 +734,7 @@
   <dimension ref="A1:E65"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.2"/>
@@ -1712,5 +1761,7 @@
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>